<commit_message>
Fixed zero amount lines
</commit_message>
<xml_diff>
--- a/TestApp/bin/Debug/net6.0-windows/Resources/Költségfelhasználás HŐ-2021-00004.xlsx
+++ b/TestApp/bin/Debug/net6.0-windows/Resources/Költségfelhasználás HŐ-2021-00004.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felhasználó\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56A2855-9A7D-4514-9451-A9FF0EE1230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8578F7FF-4B49-45FE-8DC4-AECA1AE14596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10966,11 +10966,11 @@
       </c>
       <c r="N4" s="59">
         <f>SUMIFS(Bérköltség!P7:P413,Bérköltség!C7:C413,J4,Bérköltség!I7:I413,"Köt. váll.")+SUMIFS(Bérköltség!Q7:Q413,Bérköltség!C7:C413,J4,Bérköltség!I7:I413,"Köt. váll.")+SUMIFS(Dologi_felhalm.!G42:G73,Dologi_felhalm.!B42:B73,B10,Dologi_felhalm.!H42:H73,"Köt. Váll.")</f>
-        <v>15303326</v>
+        <v>15133939</v>
       </c>
       <c r="O4" s="59">
         <f>M4-N4</f>
-        <v>113741450</v>
+        <v>113910837</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -10993,11 +10993,11 @@
       </c>
       <c r="F5" s="59">
         <f>SUMIFS(Bérköltség!$P$7:$P$413,Bérköltség!$F$7:$F$413,$B5,Bérköltség!$I$7:$I$413,"Köt. váll.")</f>
-        <v>4819443</v>
+        <v>4669543</v>
       </c>
       <c r="G5" s="59">
         <f t="shared" ref="G5" si="1">E5-F5</f>
-        <v>4160615</v>
+        <v>4310515</v>
       </c>
       <c r="I5" s="193" t="s">
         <v>36</v>
@@ -11017,11 +11017,11 @@
       </c>
       <c r="N5" s="155">
         <f>SUM(N4:N4)</f>
-        <v>15303326</v>
+        <v>15133939</v>
       </c>
       <c r="O5" s="154">
         <f>SUM(O4:O4)</f>
-        <v>113741450</v>
+        <v>113910837</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -11043,11 +11043,11 @@
       </c>
       <c r="F6" s="148">
         <f>SUM(F4:F5)</f>
-        <v>13542766</v>
+        <v>13392866</v>
       </c>
       <c r="G6" s="148">
         <f>SUM(G4:G5)</f>
-        <v>94541216</v>
+        <v>94691116</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -11109,11 +11109,11 @@
       </c>
       <c r="F8" s="59">
         <f>SUMIFS(Bérköltség!$Q$7:$Q$413,Bérköltség!$G$7:$G$413,$B8,Bérköltség!$I$7:$I$413,"Köt. váll.")</f>
-        <v>626526</v>
+        <v>607039</v>
       </c>
       <c r="G8" s="59">
         <f t="shared" si="3"/>
-        <v>1433501</v>
+        <v>1452988</v>
       </c>
       <c r="I8" s="161" t="s">
         <v>282</v>
@@ -11144,11 +11144,11 @@
       </c>
       <c r="F9" s="148">
         <f>SUM(F7:F8)</f>
-        <v>1760560</v>
+        <v>1741073</v>
       </c>
       <c r="G9" s="148">
         <f>SUM(G7:G8)</f>
-        <v>16679988</v>
+        <v>16699475</v>
       </c>
       <c r="I9" s="178" t="s">
         <v>218</v>
@@ -11246,11 +11246,11 @@
       </c>
       <c r="F12" s="152">
         <f>F6+F9+F11</f>
-        <v>15303326</v>
+        <v>15133939</v>
       </c>
       <c r="G12" s="152">
         <f>G6+G9+G11</f>
-        <v>113741450</v>
+        <v>113910837</v>
       </c>
       <c r="I12" s="161" t="s">
         <v>222</v>
@@ -11313,7 +11313,7 @@
       <selection activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-      <autoFilter ref="A3:L77" xr:uid="{29234A85-1D70-49D0-8563-FFD6BEE01285}"/>
+      <autoFilter ref="A3:L77" xr:uid="{C26FACBD-1F5B-4D88-B657-D2905B0BB209}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -11332,11 +11332,11 @@
   <dimension ref="A1:AR453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:H2"/>
+      <selection pane="bottomRight" activeCell="P187" sqref="P187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -11628,7 +11628,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38"/>
       <c r="B7" s="38" t="s">
         <v>223</v>
@@ -11705,7 +11705,7 @@
         <v>8482470434</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38"/>
       <c r="B8" s="38" t="s">
         <v>223</v>
@@ -11782,7 +11782,7 @@
         <v>8482470434</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
       <c r="B9" s="38" t="s">
         <v>223</v>
@@ -11859,7 +11859,7 @@
         <v>8482470434</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="38" t="s">
         <v>223</v>
@@ -11948,7 +11948,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="38" t="s">
         <v>223</v>
@@ -12035,7 +12035,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="38" t="s">
         <v>216</v>
@@ -12112,7 +12112,7 @@
         <v>8399050482</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="38" t="s">
         <v>216</v>
@@ -12189,7 +12189,7 @@
         <v>8399050482</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="38" t="s">
         <v>216</v>
@@ -12264,7 +12264,7 @@
         <v>8399050482</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="38" t="s">
         <v>216</v>
@@ -12339,7 +12339,7 @@
         <v>8399050482</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="38" t="s">
         <v>216</v>
@@ -12416,7 +12416,7 @@
         <v>8399050482</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38" t="s">
         <v>216</v>
@@ -12506,7 +12506,7 @@
         <v>29756</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="38" t="s">
         <v>216</v>
@@ -12594,7 +12594,7 @@
         <v>43096</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="38" t="s">
         <v>216</v>
@@ -12681,7 +12681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="38" t="s">
         <v>216</v>
@@ -12768,7 +12768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="38" t="s">
         <v>216</v>
@@ -12855,7 +12855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38"/>
       <c r="B22" s="38" t="s">
         <v>216</v>
@@ -13080,7 +13080,7 @@
         <v>8399050482</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38"/>
       <c r="B25" s="38" t="s">
         <v>192</v>
@@ -13156,7 +13156,7 @@
         <v>8459421406</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38"/>
       <c r="B26" s="38" t="s">
         <v>192</v>
@@ -13232,7 +13232,7 @@
         <v>8459421406</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38"/>
       <c r="B27" s="38" t="s">
         <v>192</v>
@@ -13308,7 +13308,7 @@
         <v>8459421406</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38"/>
       <c r="B28" s="38" t="s">
         <v>193</v>
@@ -13384,7 +13384,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38"/>
       <c r="B29" s="38" t="s">
         <v>193</v>
@@ -13460,7 +13460,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="38"/>
       <c r="B30" s="38" t="s">
         <v>193</v>
@@ -13536,7 +13536,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="38"/>
       <c r="B31" s="38" t="s">
         <v>193</v>
@@ -13612,7 +13612,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="38"/>
       <c r="B32" s="38" t="s">
         <v>193</v>
@@ -13688,7 +13688,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="33" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="38"/>
       <c r="B33" s="38" t="s">
         <v>193</v>
@@ -13764,7 +13764,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="34" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="38"/>
       <c r="B34" s="38" t="s">
         <v>193</v>
@@ -13840,7 +13840,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="35" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="38"/>
       <c r="B35" s="38" t="s">
         <v>193</v>
@@ -13916,7 +13916,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="36" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="38"/>
       <c r="B36" s="38" t="s">
         <v>193</v>
@@ -13992,7 +13992,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="37" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="38"/>
       <c r="B37" s="38" t="s">
         <v>193</v>
@@ -14081,7 +14081,7 @@
         <v>6933</v>
       </c>
     </row>
-    <row r="38" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="38"/>
       <c r="B38" s="38" t="s">
         <v>193</v>
@@ -14168,7 +14168,7 @@
         <v>17767</v>
       </c>
     </row>
-    <row r="39" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="38"/>
       <c r="B39" s="38" t="s">
         <v>193</v>
@@ -14254,7 +14254,7 @@
         <v>-10400</v>
       </c>
     </row>
-    <row r="40" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="38"/>
       <c r="B40" s="38" t="s">
         <v>193</v>
@@ -14340,7 +14340,7 @@
         <v>-10400</v>
       </c>
     </row>
-    <row r="41" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="38"/>
       <c r="B41" s="38" t="s">
         <v>193</v>
@@ -14426,7 +14426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="38"/>
       <c r="B42" s="38" t="s">
         <v>193</v>
@@ -14648,7 +14648,7 @@
         <v>8399572616</v>
       </c>
     </row>
-    <row r="45" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="38"/>
       <c r="B45" s="38" t="s">
         <v>194</v>
@@ -14725,7 +14725,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="46" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="38"/>
       <c r="B46" s="38" t="s">
         <v>194</v>
@@ -14802,7 +14802,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="47" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>
       <c r="B47" s="38" t="s">
         <v>194</v>
@@ -14879,7 +14879,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="48" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="38"/>
       <c r="B48" s="38" t="s">
         <v>194</v>
@@ -14956,7 +14956,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="49" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="38"/>
       <c r="B49" s="38" t="s">
         <v>194</v>
@@ -15033,7 +15033,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="50" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="38"/>
       <c r="B50" s="38" t="s">
         <v>194</v>
@@ -15110,7 +15110,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="51" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="38"/>
       <c r="B51" s="38" t="s">
         <v>194</v>
@@ -15187,7 +15187,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="52" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="38"/>
       <c r="B52" s="38" t="s">
         <v>194</v>
@@ -15264,7 +15264,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="53" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="38"/>
       <c r="B53" s="38" t="s">
         <v>194</v>
@@ -15341,7 +15341,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="54" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="38"/>
       <c r="B54" s="38" t="s">
         <v>194</v>
@@ -15431,7 +15431,7 @@
         <v>27238</v>
       </c>
     </row>
-    <row r="55" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="38"/>
       <c r="B55" s="38" t="s">
         <v>194</v>
@@ -15519,7 +15519,7 @@
         <v>44262</v>
       </c>
     </row>
-    <row r="56" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="38"/>
       <c r="B56" s="173" t="s">
         <v>194</v>
@@ -15606,7 +15606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="38"/>
       <c r="B57" s="173" t="s">
         <v>194</v>
@@ -15693,7 +15693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="38"/>
       <c r="B58" s="173" t="s">
         <v>194</v>
@@ -15780,7 +15780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="38"/>
       <c r="B59" s="173" t="s">
         <v>194</v>
@@ -16005,7 +16005,7 @@
         <v>8396372314</v>
       </c>
     </row>
-    <row r="62" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="38"/>
       <c r="B62" s="38" t="s">
         <v>200</v>
@@ -16082,7 +16082,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="63" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="38"/>
       <c r="B63" s="38" t="s">
         <v>200</v>
@@ -16159,7 +16159,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="64" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="38"/>
       <c r="B64" s="38" t="s">
         <v>200</v>
@@ -16236,7 +16236,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="65" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="38"/>
       <c r="B65" s="38" t="s">
         <v>200</v>
@@ -16313,7 +16313,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="66" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="38"/>
       <c r="B66" s="38" t="s">
         <v>200</v>
@@ -16390,7 +16390,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="67" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="38"/>
       <c r="B67" s="38" t="s">
         <v>200</v>
@@ -16467,7 +16467,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="68" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="38"/>
       <c r="B68" s="38" t="s">
         <v>200</v>
@@ -16544,7 +16544,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="69" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="38"/>
       <c r="B69" s="38" t="s">
         <v>200</v>
@@ -16621,7 +16621,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="70" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="38"/>
       <c r="B70" s="38" t="s">
         <v>200</v>
@@ -16711,7 +16711,7 @@
         <v>28841</v>
       </c>
     </row>
-    <row r="71" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="38"/>
       <c r="B71" s="38" t="s">
         <v>200</v>
@@ -16799,7 +16799,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="72" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="38"/>
       <c r="B72" s="38" t="s">
         <v>200</v>
@@ -16886,7 +16886,7 @@
         <v>3445</v>
       </c>
     </row>
-    <row r="73" spans="1:29" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="38"/>
       <c r="B73" s="38" t="s">
         <v>200</v>
@@ -16973,7 +16973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="38"/>
       <c r="B74" s="38" t="s">
         <v>200</v>
@@ -17060,7 +17060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="38"/>
       <c r="B75" s="38" t="s">
         <v>200</v>
@@ -17285,7 +17285,7 @@
         <v>8426043291</v>
       </c>
     </row>
-    <row r="78" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="38"/>
       <c r="B78" s="38" t="s">
         <v>188</v>
@@ -17361,7 +17361,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="79" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="38"/>
       <c r="B79" s="38" t="s">
         <v>188</v>
@@ -17437,7 +17437,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="80" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="38"/>
       <c r="B80" s="38" t="s">
         <v>188</v>
@@ -17513,7 +17513,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="81" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="38"/>
       <c r="B81" s="38" t="s">
         <v>188</v>
@@ -17589,7 +17589,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="82" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="38"/>
       <c r="B82" s="38" t="s">
         <v>188</v>
@@ -17665,7 +17665,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="83" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="38"/>
       <c r="B83" s="38" t="s">
         <v>188</v>
@@ -17741,7 +17741,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="84" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="38"/>
       <c r="B84" s="38" t="s">
         <v>188</v>
@@ -17817,7 +17817,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="85" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="38"/>
       <c r="B85" s="38" t="s">
         <v>188</v>
@@ -17891,7 +17891,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="86" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="38"/>
       <c r="B86" s="38" t="s">
         <v>188</v>
@@ -17967,7 +17967,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="87" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="38"/>
       <c r="B87" s="38" t="s">
         <v>188</v>
@@ -18043,7 +18043,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="88" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="38"/>
       <c r="B88" s="38" t="s">
         <v>188</v>
@@ -18132,7 +18132,7 @@
         <v>52990</v>
       </c>
     </row>
-    <row r="89" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="38"/>
       <c r="B89" s="38" t="s">
         <v>188</v>
@@ -18219,7 +18219,7 @@
         <v>86110</v>
       </c>
     </row>
-    <row r="90" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="38"/>
       <c r="B90" s="38" t="s">
         <v>188</v>
@@ -18305,7 +18305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="38"/>
       <c r="B91" s="38" t="s">
         <v>188</v>
@@ -18391,7 +18391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="38"/>
       <c r="B92" s="38" t="s">
         <v>188</v>
@@ -18477,7 +18477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="38"/>
       <c r="B93" s="38" t="s">
         <v>188</v>
@@ -18699,7 +18699,7 @@
         <v>8405671307</v>
       </c>
     </row>
-    <row r="96" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="38"/>
       <c r="B96" s="38" t="s">
         <v>224</v>
@@ -18774,7 +18774,7 @@
         <v>8462721202</v>
       </c>
     </row>
-    <row r="97" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="38"/>
       <c r="B97" s="38" t="s">
         <v>224</v>
@@ -18849,7 +18849,7 @@
         <v>8462721202</v>
       </c>
     </row>
-    <row r="98" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="38"/>
       <c r="B98" s="38" t="s">
         <v>224</v>
@@ -18926,7 +18926,7 @@
         <v>8462721202</v>
       </c>
     </row>
-    <row r="99" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="38"/>
       <c r="B99" s="38" t="s">
         <v>224</v>
@@ -19016,7 +19016,7 @@
         <v>30051</v>
       </c>
     </row>
-    <row r="100" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="38"/>
       <c r="B100" s="38" t="s">
         <v>224</v>
@@ -19104,7 +19104,7 @@
         <v>47793</v>
       </c>
     </row>
-    <row r="101" spans="1:29" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:29" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="38"/>
       <c r="B101" s="38" t="s">
         <v>224</v>
@@ -19191,7 +19191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="38"/>
       <c r="B102" s="38" t="s">
         <v>224</v>
@@ -19278,7 +19278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="38"/>
       <c r="B103" s="38" t="s">
         <v>224</v>
@@ -19365,7 +19365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="38"/>
       <c r="B104" s="38" t="s">
         <v>224</v>
@@ -19890,7 +19890,7 @@
         <v>8462721202</v>
       </c>
     </row>
-    <row r="111" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="38"/>
       <c r="B111" s="38" t="s">
         <v>199</v>
@@ -19967,7 +19967,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="112" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="38"/>
       <c r="B112" s="38" t="s">
         <v>199</v>
@@ -20044,7 +20044,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="113" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="38"/>
       <c r="B113" s="38" t="s">
         <v>199</v>
@@ -20121,7 +20121,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="114" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="38"/>
       <c r="B114" s="38" t="s">
         <v>199</v>
@@ -20198,7 +20198,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="115" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="38"/>
       <c r="B115" s="38" t="s">
         <v>199</v>
@@ -20275,7 +20275,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="116" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="38"/>
       <c r="B116" s="38" t="s">
         <v>199</v>
@@ -20352,7 +20352,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="117" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="38"/>
       <c r="B117" s="38" t="s">
         <v>199</v>
@@ -20427,7 +20427,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="118" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="38"/>
       <c r="B118" s="38" t="s">
         <v>199</v>
@@ -20502,7 +20502,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="119" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="38"/>
       <c r="B119" s="38" t="s">
         <v>199</v>
@@ -20577,7 +20577,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="120" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="38"/>
       <c r="B120" s="38" t="s">
         <v>199</v>
@@ -20665,7 +20665,7 @@
         <v>77178</v>
       </c>
     </row>
-    <row r="121" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="38"/>
       <c r="B121" s="38" t="s">
         <v>199</v>
@@ -20751,7 +20751,7 @@
         <v>118849</v>
       </c>
     </row>
-    <row r="122" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="38"/>
       <c r="B122" s="38" t="s">
         <v>199</v>
@@ -20838,7 +20838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="38"/>
       <c r="B123" s="38" t="s">
         <v>199</v>
@@ -20925,7 +20925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="38"/>
       <c r="B124" s="38" t="s">
         <v>199</v>
@@ -21012,7 +21012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="38"/>
       <c r="B125" s="38" t="s">
         <v>199</v>
@@ -21162,7 +21162,7 @@
         <v>8438731872</v>
       </c>
     </row>
-    <row r="127" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="38"/>
       <c r="B127" s="38" t="s">
         <v>189</v>
@@ -21239,7 +21239,7 @@
         <v>8430140549</v>
       </c>
     </row>
-    <row r="128" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="38"/>
       <c r="B128" s="173" t="s">
         <v>189</v>
@@ -21461,7 +21461,7 @@
         <v>8430140549</v>
       </c>
     </row>
-    <row r="131" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="38"/>
       <c r="B131" s="38" t="s">
         <v>190</v>
@@ -21538,7 +21538,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="132" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="38"/>
       <c r="B132" s="38" t="s">
         <v>190</v>
@@ -21615,7 +21615,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="133" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="38"/>
       <c r="B133" s="38" t="s">
         <v>190</v>
@@ -21692,7 +21692,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="134" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="38"/>
       <c r="B134" s="38" t="s">
         <v>190</v>
@@ -21769,7 +21769,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="135" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="38"/>
       <c r="B135" s="38" t="s">
         <v>190</v>
@@ -21846,7 +21846,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="136" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="38"/>
       <c r="B136" s="38" t="s">
         <v>190</v>
@@ -21921,7 +21921,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="137" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="38"/>
       <c r="B137" s="38" t="s">
         <v>190</v>
@@ -21996,7 +21996,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="138" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="38"/>
       <c r="B138" s="38" t="s">
         <v>190</v>
@@ -22071,7 +22071,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="139" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="38"/>
       <c r="B139" s="38" t="s">
         <v>190</v>
@@ -22146,7 +22146,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="140" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="38"/>
       <c r="B140" s="38" t="s">
         <v>190</v>
@@ -22221,7 +22221,7 @@
         <v>8477941602</v>
       </c>
     </row>
-    <row r="141" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="38"/>
       <c r="B141" s="38" t="s">
         <v>190</v>
@@ -22309,7 +22309,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="142" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="38"/>
       <c r="B142" s="38" t="s">
         <v>190</v>
@@ -22395,7 +22395,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="38"/>
       <c r="B143" s="38" t="s">
         <v>195</v>
@@ -22472,7 +22472,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="144" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="38"/>
       <c r="B144" s="38" t="s">
         <v>195</v>
@@ -22549,7 +22549,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="145" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="38"/>
       <c r="B145" s="38" t="s">
         <v>195</v>
@@ -22626,7 +22626,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="146" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="38"/>
       <c r="B146" s="38" t="s">
         <v>195</v>
@@ -22703,7 +22703,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="147" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="38"/>
       <c r="B147" s="38" t="s">
         <v>195</v>
@@ -22780,7 +22780,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="148" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="38"/>
       <c r="B148" s="38" t="s">
         <v>195</v>
@@ -22857,7 +22857,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="149" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="38"/>
       <c r="B149" s="38" t="s">
         <v>195</v>
@@ -22934,7 +22934,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="150" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="38"/>
       <c r="B150" s="38" t="s">
         <v>195</v>
@@ -23011,7 +23011,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="151" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="38"/>
       <c r="B151" s="38" t="s">
         <v>195</v>
@@ -23088,7 +23088,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="152" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="38"/>
       <c r="B152" s="38" t="s">
         <v>195</v>
@@ -23178,7 +23178,7 @@
         <v>16869</v>
       </c>
     </row>
-    <row r="153" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="38"/>
       <c r="B153" s="38" t="s">
         <v>195</v>
@@ -23266,7 +23266,7 @@
         <v>26773</v>
       </c>
     </row>
-    <row r="154" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="38"/>
       <c r="B154" s="38" t="s">
         <v>195</v>
@@ -23353,7 +23353,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="155" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="38"/>
       <c r="B155" s="38" t="s">
         <v>195</v>
@@ -23440,7 +23440,7 @@
         <v>-5219</v>
       </c>
     </row>
-    <row r="156" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="38"/>
       <c r="B156" s="38" t="s">
         <v>195</v>
@@ -23527,7 +23527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="38"/>
       <c r="B157" s="38" t="s">
         <v>195</v>
@@ -23752,7 +23752,7 @@
         <v>8354163245</v>
       </c>
     </row>
-    <row r="160" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="38"/>
       <c r="B160" s="38" t="s">
         <v>198</v>
@@ -23830,7 +23830,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="161" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="38"/>
       <c r="B161" s="38" t="s">
         <v>198</v>
@@ -23906,7 +23906,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="162" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="38"/>
       <c r="B162" s="38" t="s">
         <v>198</v>
@@ -23982,7 +23982,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="163" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="38"/>
       <c r="B163" s="38" t="s">
         <v>198</v>
@@ -24058,7 +24058,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="164" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="38"/>
       <c r="B164" s="38" t="s">
         <v>198</v>
@@ -24134,7 +24134,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="165" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="38"/>
       <c r="B165" s="38" t="s">
         <v>198</v>
@@ -24210,7 +24210,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="166" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="38"/>
       <c r="B166" s="38" t="s">
         <v>198</v>
@@ -24286,7 +24286,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="167" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="38"/>
       <c r="B167" s="38" t="s">
         <v>198</v>
@@ -24362,7 +24362,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="168" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="38"/>
       <c r="B168" s="38" t="s">
         <v>198</v>
@@ -24438,7 +24438,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="169" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="38"/>
       <c r="B169" s="38" t="s">
         <v>198</v>
@@ -24528,7 +24528,7 @@
         <v>34436</v>
       </c>
     </row>
-    <row r="170" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="38"/>
       <c r="B170" s="38" t="s">
         <v>198</v>
@@ -24616,7 +24616,7 @@
         <v>51377</v>
       </c>
     </row>
-    <row r="171" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="38"/>
       <c r="B171" s="38" t="s">
         <v>198</v>
@@ -24702,7 +24702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="38"/>
       <c r="B172" s="38" t="s">
         <v>198</v>
@@ -24788,7 +24788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="38"/>
       <c r="B173" s="38" t="s">
         <v>198</v>
@@ -24874,7 +24874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="38"/>
       <c r="B174" s="38" t="s">
         <v>198</v>
@@ -24921,15 +24921,14 @@
         <v>0.25287356321839083</v>
       </c>
       <c r="P174" s="80">
-        <v>150000</v>
+        <v>100</v>
       </c>
       <c r="Q174" s="80">
-        <f t="shared" si="130"/>
-        <v>19500</v>
+        <v>13</v>
       </c>
       <c r="R174" s="159">
         <f t="shared" si="131"/>
-        <v>4.4057812074582425E-3</v>
+        <v>0.25270791803038356</v>
       </c>
       <c r="S174" s="113">
         <v>0.13</v>
@@ -25096,7 +25095,7 @@
         <v>8381490405</v>
       </c>
     </row>
-    <row r="177" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="38"/>
       <c r="B177" s="38" t="s">
         <v>215</v>
@@ -25173,7 +25172,7 @@
         <v>8419653322</v>
       </c>
     </row>
-    <row r="178" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="38"/>
       <c r="B178" s="38" t="s">
         <v>215</v>
@@ -25250,7 +25249,7 @@
         <v>8419653322</v>
       </c>
     </row>
-    <row r="179" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="38"/>
       <c r="B179" s="38" t="s">
         <v>215</v>
@@ -25327,7 +25326,7 @@
         <v>8419653322</v>
       </c>
     </row>
-    <row r="180" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="38"/>
       <c r="B180" s="38" t="s">
         <v>215</v>
@@ -25404,7 +25403,7 @@
         <v>8419653322</v>
       </c>
     </row>
-    <row r="181" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="38"/>
       <c r="B181" s="38" t="s">
         <v>215</v>
@@ -25481,7 +25480,7 @@
         <v>8419653322</v>
       </c>
     </row>
-    <row r="182" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="38"/>
       <c r="B182" s="38" t="s">
         <v>215</v>
@@ -25571,7 +25570,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="183" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="38"/>
       <c r="B183" s="38" t="s">
         <v>215</v>
@@ -25659,7 +25658,7 @@
         <v>51080</v>
       </c>
     </row>
-    <row r="184" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="38"/>
       <c r="B184" s="38" t="s">
         <v>215</v>
@@ -25746,7 +25745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="38"/>
       <c r="B185" s="38" t="s">
         <v>215</v>
@@ -25833,7 +25832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="38"/>
       <c r="B186" s="38" t="s">
         <v>215</v>
@@ -25920,7 +25919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="38"/>
       <c r="B187" s="38" t="s">
         <v>215</v>
@@ -26145,7 +26144,7 @@
         <v>8419653322</v>
       </c>
     </row>
-    <row r="190" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="38"/>
       <c r="B190" s="38" t="s">
         <v>184</v>
@@ -26222,7 +26221,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="191" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="38"/>
       <c r="B191" s="38" t="s">
         <v>184</v>
@@ -26299,7 +26298,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="192" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="38"/>
       <c r="B192" s="38" t="s">
         <v>184</v>
@@ -26376,7 +26375,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="193" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="38"/>
       <c r="B193" s="38" t="s">
         <v>184</v>
@@ -26453,7 +26452,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="194" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="38"/>
       <c r="B194" s="38" t="s">
         <v>184</v>
@@ -26530,7 +26529,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="195" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="38"/>
       <c r="B195" s="38" t="s">
         <v>184</v>
@@ -26607,7 +26606,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="196" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="38"/>
       <c r="B196" s="38" t="s">
         <v>184</v>
@@ -26684,7 +26683,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="197" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="38"/>
       <c r="B197" s="38" t="s">
         <v>184</v>
@@ -26761,7 +26760,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="198" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="38"/>
       <c r="B198" s="38" t="s">
         <v>184</v>
@@ -26838,7 +26837,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="199" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="38"/>
       <c r="B199" s="38" t="s">
         <v>184</v>
@@ -26915,7 +26914,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="200" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="38"/>
       <c r="B200" s="38" t="s">
         <v>184</v>
@@ -27005,7 +27004,7 @@
         <v>37732</v>
       </c>
     </row>
-    <row r="201" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="38"/>
       <c r="B201" s="38" t="s">
         <v>184</v>
@@ -27093,7 +27092,7 @@
         <v>57220</v>
       </c>
     </row>
-    <row r="202" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="38"/>
       <c r="B202" s="38" t="s">
         <v>184</v>
@@ -27180,7 +27179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="38"/>
       <c r="B203" s="38" t="s">
         <v>184</v>
@@ -27267,7 +27266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="38"/>
       <c r="B204" s="38" t="s">
         <v>184</v>
@@ -27354,7 +27353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="38"/>
       <c r="B205" s="38" t="s">
         <v>184</v>
@@ -27579,7 +27578,7 @@
         <v>8415163150</v>
       </c>
     </row>
-    <row r="208" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="38"/>
       <c r="B208" s="38" t="s">
         <v>197</v>
@@ -27656,7 +27655,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="209" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="38"/>
       <c r="B209" s="38" t="s">
         <v>197</v>
@@ -27733,7 +27732,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="210" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="38"/>
       <c r="B210" s="38" t="s">
         <v>197</v>
@@ -27810,7 +27809,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="211" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="38"/>
       <c r="B211" s="38" t="s">
         <v>197</v>
@@ -27887,7 +27886,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="212" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="38"/>
       <c r="B212" s="38" t="s">
         <v>197</v>
@@ -27964,7 +27963,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="213" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="38"/>
       <c r="B213" s="38" t="s">
         <v>197</v>
@@ -28041,7 +28040,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="214" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="38"/>
       <c r="B214" s="38" t="s">
         <v>197</v>
@@ -28118,7 +28117,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="215" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="38"/>
       <c r="B215" s="38" t="s">
         <v>197</v>
@@ -28195,7 +28194,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="216" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="38"/>
       <c r="B216" s="38" t="s">
         <v>197</v>
@@ -28272,7 +28271,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="217" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="38"/>
       <c r="B217" s="38" t="s">
         <v>197</v>
@@ -28362,7 +28361,7 @@
         <v>24987</v>
       </c>
     </row>
-    <row r="218" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="38"/>
       <c r="B218" s="38" t="s">
         <v>197</v>
@@ -28450,7 +28449,7 @@
         <v>36191</v>
       </c>
     </row>
-    <row r="219" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="38"/>
       <c r="B219" s="38" t="s">
         <v>197</v>
@@ -28537,7 +28536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="38"/>
       <c r="B220" s="38" t="s">
         <v>197</v>
@@ -28624,7 +28623,7 @@
         <v>4059</v>
       </c>
     </row>
-    <row r="221" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="38"/>
       <c r="B221" s="38" t="s">
         <v>197</v>
@@ -28711,7 +28710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="38"/>
       <c r="B222" s="38" t="s">
         <v>197</v>
@@ -28927,7 +28926,7 @@
         <v>8370633390</v>
       </c>
     </row>
-    <row r="225" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="38"/>
       <c r="B225" s="38" t="s">
         <v>202</v>
@@ -29004,7 +29003,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="226" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="38"/>
       <c r="B226" s="38" t="s">
         <v>202</v>
@@ -29081,7 +29080,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="227" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="38"/>
       <c r="B227" s="38" t="s">
         <v>202</v>
@@ -29158,7 +29157,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="228" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="38"/>
       <c r="B228" s="38" t="s">
         <v>202</v>
@@ -29235,7 +29234,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="229" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="38"/>
       <c r="B229" s="38" t="s">
         <v>202</v>
@@ -29312,7 +29311,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="230" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="38"/>
       <c r="B230" s="38" t="s">
         <v>202</v>
@@ -29389,7 +29388,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="231" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="38"/>
       <c r="B231" s="38" t="s">
         <v>202</v>
@@ -29466,7 +29465,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="232" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="38"/>
       <c r="B232" s="38" t="s">
         <v>202</v>
@@ -29543,7 +29542,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="233" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="38"/>
       <c r="B233" s="38" t="s">
         <v>202</v>
@@ -29633,7 +29632,7 @@
         <v>17720</v>
       </c>
     </row>
-    <row r="234" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="38"/>
       <c r="B234" s="38" t="s">
         <v>202</v>
@@ -29721,7 +29720,7 @@
         <v>28794</v>
       </c>
     </row>
-    <row r="235" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="38"/>
       <c r="B235" s="38" t="s">
         <v>202</v>
@@ -29808,7 +29807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="38"/>
       <c r="B236" s="38" t="s">
         <v>202</v>
@@ -29895,7 +29894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="38"/>
       <c r="B237" s="38" t="s">
         <v>202</v>
@@ -29982,7 +29981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="38"/>
       <c r="B238" s="38" t="s">
         <v>202</v>
@@ -30207,7 +30206,7 @@
         <v>8338131113</v>
       </c>
     </row>
-    <row r="241" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="38"/>
       <c r="B241" s="38" t="s">
         <v>178</v>
@@ -30284,7 +30283,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="242" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="38"/>
       <c r="B242" s="38" t="s">
         <v>178</v>
@@ -30359,7 +30358,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="243" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="38"/>
       <c r="B243" s="38" t="s">
         <v>178</v>
@@ -30434,7 +30433,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="244" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="38"/>
       <c r="B244" s="38" t="s">
         <v>178</v>
@@ -30509,7 +30508,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="245" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="38"/>
       <c r="B245" s="38" t="s">
         <v>178</v>
@@ -30585,7 +30584,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="246" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="38"/>
       <c r="B246" s="38" t="s">
         <v>178</v>
@@ -30661,7 +30660,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="247" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="38"/>
       <c r="B247" s="38" t="s">
         <v>178</v>
@@ -30737,7 +30736,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="248" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="38"/>
       <c r="B248" s="38" t="s">
         <v>178</v>
@@ -30813,7 +30812,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="249" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="38"/>
       <c r="B249" s="38" t="s">
         <v>178</v>
@@ -30889,7 +30888,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="250" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="38"/>
       <c r="B250" s="38" t="s">
         <v>178</v>
@@ -30965,7 +30964,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="251" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="38"/>
       <c r="B251" s="38" t="s">
         <v>178</v>
@@ -31054,7 +31053,7 @@
         <v>8537.6190476190459</v>
       </c>
     </row>
-    <row r="252" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="38"/>
       <c r="B252" s="38" t="s">
         <v>178</v>
@@ -31141,7 +31140,7 @@
         <v>18767.380952380954</v>
       </c>
     </row>
-    <row r="253" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="38"/>
       <c r="B253" s="38" t="s">
         <v>178</v>
@@ -31227,7 +31226,7 @@
         <v>-6530</v>
       </c>
     </row>
-    <row r="254" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="38"/>
       <c r="B254" s="38" t="s">
         <v>178</v>
@@ -31313,7 +31312,7 @@
         <v>-6530</v>
       </c>
     </row>
-    <row r="255" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="38"/>
       <c r="B255" s="38" t="s">
         <v>178</v>
@@ -31399,7 +31398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="38"/>
       <c r="B256" s="38" t="s">
         <v>178</v>
@@ -31624,7 +31623,7 @@
         <v>8448150856</v>
       </c>
     </row>
-    <row r="259" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="38"/>
       <c r="B259" s="38" t="s">
         <v>196</v>
@@ -31701,7 +31700,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="260" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="38"/>
       <c r="B260" s="38" t="s">
         <v>196</v>
@@ -31778,7 +31777,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="261" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="38"/>
       <c r="B261" s="38" t="s">
         <v>196</v>
@@ -31855,7 +31854,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="262" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="38"/>
       <c r="B262" s="38" t="s">
         <v>196</v>
@@ -31932,7 +31931,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="263" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="38"/>
       <c r="B263" s="38" t="s">
         <v>196</v>
@@ -32009,7 +32008,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="264" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="38"/>
       <c r="B264" s="38" t="s">
         <v>196</v>
@@ -32086,7 +32085,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="265" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="38"/>
       <c r="B265" s="38" t="s">
         <v>196</v>
@@ -32163,7 +32162,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="266" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="38"/>
       <c r="B266" s="38" t="s">
         <v>196</v>
@@ -32240,7 +32239,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="267" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="38"/>
       <c r="B267" s="38" t="s">
         <v>196</v>
@@ -32317,7 +32316,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="268" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="38"/>
       <c r="B268" s="38" t="s">
         <v>196</v>
@@ -32407,7 +32406,7 @@
         <v>33521</v>
       </c>
     </row>
-    <row r="269" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="38"/>
       <c r="B269" s="38" t="s">
         <v>196</v>
@@ -32495,7 +32494,7 @@
         <v>51629</v>
       </c>
     </row>
-    <row r="270" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="38"/>
       <c r="B270" s="38" t="s">
         <v>196</v>
@@ -32582,7 +32581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="38"/>
       <c r="B271" s="38" t="s">
         <v>196</v>
@@ -32669,7 +32668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="38"/>
       <c r="B272" s="38" t="s">
         <v>196</v>
@@ -32755,7 +32754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="38"/>
       <c r="B273" s="38" t="s">
         <v>196</v>
@@ -32977,7 +32976,7 @@
         <v>8410460823</v>
       </c>
     </row>
-    <row r="276" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="38"/>
       <c r="B276" s="38" t="s">
         <v>185</v>
@@ -33054,7 +33053,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="277" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="38"/>
       <c r="B277" s="38" t="s">
         <v>185</v>
@@ -33131,7 +33130,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="278" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="38"/>
       <c r="B278" s="38" t="s">
         <v>185</v>
@@ -33208,7 +33207,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="279" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="38"/>
       <c r="B279" s="38" t="s">
         <v>185</v>
@@ -33285,7 +33284,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="280" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="38"/>
       <c r="B280" s="38" t="s">
         <v>185</v>
@@ -33362,7 +33361,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="281" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="38"/>
       <c r="B281" s="38" t="s">
         <v>185</v>
@@ -33439,7 +33438,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="282" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="38"/>
       <c r="B282" s="38" t="s">
         <v>185</v>
@@ -33516,7 +33515,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="283" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="38"/>
       <c r="B283" s="38" t="s">
         <v>185</v>
@@ -33593,7 +33592,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="284" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="38"/>
       <c r="B284" s="38" t="s">
         <v>185</v>
@@ -33670,7 +33669,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="285" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="38"/>
       <c r="B285" s="38" t="s">
         <v>185</v>
@@ -33747,7 +33746,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="286" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="38"/>
       <c r="B286" s="38" t="s">
         <v>185</v>
@@ -33837,7 +33836,7 @@
         <v>67105</v>
       </c>
     </row>
-    <row r="287" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="38"/>
       <c r="B287" s="38" t="s">
         <v>185</v>
@@ -33925,7 +33924,7 @@
         <v>109045</v>
       </c>
     </row>
-    <row r="288" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="38"/>
       <c r="B288" s="38" t="s">
         <v>185</v>
@@ -34012,7 +34011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="38"/>
       <c r="B289" s="38" t="s">
         <v>185</v>
@@ -34099,7 +34098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="38"/>
       <c r="B290" s="38" t="s">
         <v>185</v>
@@ -34186,7 +34185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="38"/>
       <c r="B291" s="173" t="s">
         <v>185</v>
@@ -34411,7 +34410,7 @@
         <v>8421732463</v>
       </c>
     </row>
-    <row r="294" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="38"/>
       <c r="B294" s="38" t="s">
         <v>201</v>
@@ -34487,7 +34486,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="295" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="38"/>
       <c r="B295" s="38" t="s">
         <v>201</v>
@@ -34563,7 +34562,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="296" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="38"/>
       <c r="B296" s="38" t="s">
         <v>201</v>
@@ -34639,7 +34638,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="297" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="38"/>
       <c r="B297" s="38" t="s">
         <v>201</v>
@@ -34715,7 +34714,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="298" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="38"/>
       <c r="B298" s="38" t="s">
         <v>201</v>
@@ -34791,7 +34790,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="299" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="38"/>
       <c r="B299" s="38" t="s">
         <v>201</v>
@@ -34867,7 +34866,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="300" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="38"/>
       <c r="B300" s="38" t="s">
         <v>201</v>
@@ -34943,7 +34942,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="301" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="38"/>
       <c r="B301" s="38" t="s">
         <v>201</v>
@@ -35019,7 +35018,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="302" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="38"/>
       <c r="B302" s="38" t="s">
         <v>201</v>
@@ -35108,7 +35107,7 @@
         <v>40865</v>
       </c>
     </row>
-    <row r="303" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="38"/>
       <c r="B303" s="38" t="s">
         <v>201</v>
@@ -35195,7 +35194,7 @@
         <v>62927</v>
       </c>
     </row>
-    <row r="304" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="38"/>
       <c r="B304" s="38" t="s">
         <v>201</v>
@@ -35281,7 +35280,7 @@
         <v>6697</v>
       </c>
     </row>
-    <row r="305" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="38"/>
       <c r="B305" s="38" t="s">
         <v>201</v>
@@ -35367,7 +35366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="38"/>
       <c r="B306" s="38" t="s">
         <v>201</v>
@@ -35453,7 +35452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="38"/>
       <c r="B307" s="38" t="s">
         <v>201</v>
@@ -35677,7 +35676,7 @@
         <v>8396223912</v>
       </c>
     </row>
-    <row r="310" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="38"/>
       <c r="B310" s="38" t="s">
         <v>181</v>
@@ -35754,7 +35753,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="311" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="38"/>
       <c r="B311" s="38" t="s">
         <v>181</v>
@@ -35829,7 +35828,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="312" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="38"/>
       <c r="B312" s="38" t="s">
         <v>181</v>
@@ -35904,7 +35903,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="313" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="38"/>
       <c r="B313" s="38" t="s">
         <v>181</v>
@@ -35979,7 +35978,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="314" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="38"/>
       <c r="B314" s="38" t="s">
         <v>181</v>
@@ -36054,7 +36053,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="315" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="38"/>
       <c r="B315" s="38" t="s">
         <v>181</v>
@@ -36129,7 +36128,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="316" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="38"/>
       <c r="B316" s="38" t="s">
         <v>181</v>
@@ -36204,7 +36203,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="317" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="38"/>
       <c r="B317" s="173" t="s">
         <v>181</v>
@@ -36279,7 +36278,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="318" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="38"/>
       <c r="B318" s="173" t="s">
         <v>181</v>
@@ -36354,7 +36353,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="319" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="38"/>
       <c r="B319" s="173" t="s">
         <v>181</v>
@@ -36429,7 +36428,7 @@
         <v>8488690673</v>
       </c>
     </row>
-    <row r="320" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="38"/>
       <c r="B320" s="173" t="s">
         <v>181</v>
@@ -36517,7 +36516,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="321" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="38"/>
       <c r="B321" s="173" t="s">
         <v>181</v>
@@ -36603,7 +36602,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="322" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="38"/>
       <c r="B322" s="173" t="s">
         <v>181</v>
@@ -36688,7 +36687,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="323" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="38"/>
       <c r="B323" s="173" t="s">
         <v>181</v>
@@ -36775,7 +36774,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="324" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="38"/>
       <c r="B324" s="38" t="s">
         <v>214</v>
@@ -36853,7 +36852,7 @@
         <v>8397324542</v>
       </c>
     </row>
-    <row r="325" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="38"/>
       <c r="B325" s="38" t="s">
         <v>214</v>
@@ -36931,7 +36930,7 @@
         <v>8397324542</v>
       </c>
     </row>
-    <row r="326" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="38"/>
       <c r="B326" s="38" t="s">
         <v>214</v>
@@ -37009,7 +37008,7 @@
         <v>8397324542</v>
       </c>
     </row>
-    <row r="327" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="38"/>
       <c r="B327" s="38" t="s">
         <v>214</v>
@@ -37087,7 +37086,7 @@
         <v>8397324542</v>
       </c>
     </row>
-    <row r="328" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="38"/>
       <c r="B328" s="38" t="s">
         <v>214</v>
@@ -37165,7 +37164,7 @@
         <v>8397324542</v>
       </c>
     </row>
-    <row r="329" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="38"/>
       <c r="B329" s="38" t="s">
         <v>214</v>
@@ -37255,7 +37254,7 @@
         <v>64071</v>
       </c>
     </row>
-    <row r="330" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="38"/>
       <c r="B330" s="38" t="s">
         <v>214</v>
@@ -37343,7 +37342,7 @@
         <v>91929</v>
       </c>
     </row>
-    <row r="331" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="38"/>
       <c r="B331" s="38" t="s">
         <v>214</v>
@@ -37431,7 +37430,7 @@
         <v>19500</v>
       </c>
     </row>
-    <row r="332" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="38"/>
       <c r="B332" s="38" t="s">
         <v>214</v>
@@ -37519,7 +37518,7 @@
         <v>19500</v>
       </c>
     </row>
-    <row r="333" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="38"/>
       <c r="B333" s="38" t="s">
         <v>214</v>
@@ -37607,7 +37606,7 @@
         <v>19500</v>
       </c>
     </row>
-    <row r="334" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="38"/>
       <c r="B334" s="38" t="s">
         <v>214</v>
@@ -37826,7 +37825,7 @@
         <v>8397324542</v>
       </c>
     </row>
-    <row r="337" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="38"/>
       <c r="B337" s="38" t="s">
         <v>186</v>
@@ -37903,7 +37902,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="338" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="38"/>
       <c r="B338" s="38" t="s">
         <v>186</v>
@@ -37980,7 +37979,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="339" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="38"/>
       <c r="B339" s="38" t="s">
         <v>186</v>
@@ -38057,7 +38056,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="340" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="38"/>
       <c r="B340" s="38" t="s">
         <v>186</v>
@@ -38134,7 +38133,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="341" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="38"/>
       <c r="B341" s="38" t="s">
         <v>186</v>
@@ -38211,7 +38210,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="342" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="38"/>
       <c r="B342" s="38" t="s">
         <v>186</v>
@@ -38288,7 +38287,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="343" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="38"/>
       <c r="B343" s="38" t="s">
         <v>186</v>
@@ -38365,7 +38364,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="344" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="38"/>
       <c r="B344" s="38" t="s">
         <v>186</v>
@@ -38437,7 +38436,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="345" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="38"/>
       <c r="B345" s="38" t="s">
         <v>186</v>
@@ -38514,7 +38513,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="346" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="38"/>
       <c r="B346" s="38" t="s">
         <v>186</v>
@@ -38591,7 +38590,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="347" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="38"/>
       <c r="B347" s="38" t="s">
         <v>186</v>
@@ -38681,7 +38680,7 @@
         <v>51010</v>
       </c>
     </row>
-    <row r="348" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="38"/>
       <c r="B348" s="38" t="s">
         <v>186</v>
@@ -38769,7 +38768,7 @@
         <v>82890</v>
       </c>
     </row>
-    <row r="349" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="38"/>
       <c r="B349" s="38" t="s">
         <v>186</v>
@@ -38854,7 +38853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="38"/>
       <c r="B350" s="38" t="s">
         <v>186</v>
@@ -38939,7 +38938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="38"/>
       <c r="B351" s="38" t="s">
         <v>186</v>
@@ -39026,7 +39025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="38"/>
       <c r="B352" s="173" t="s">
         <v>186</v>
@@ -39176,7 +39175,7 @@
         <v>8372793190</v>
       </c>
     </row>
-    <row r="354" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="38"/>
       <c r="B354" s="38" t="s">
         <v>191</v>
@@ -39252,7 +39251,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="355" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="38"/>
       <c r="B355" s="38" t="s">
         <v>191</v>
@@ -39329,7 +39328,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="356" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="38"/>
       <c r="B356" s="38" t="s">
         <v>191</v>
@@ -39406,7 +39405,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="357" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="38"/>
       <c r="B357" s="38" t="s">
         <v>191</v>
@@ -39483,7 +39482,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="358" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="38"/>
       <c r="B358" s="38" t="s">
         <v>191</v>
@@ -39560,7 +39559,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="359" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="38"/>
       <c r="B359" s="38" t="s">
         <v>191</v>
@@ -39636,7 +39635,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="360" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="38"/>
       <c r="B360" s="38" t="s">
         <v>191</v>
@@ -39712,7 +39711,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="361" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="38"/>
       <c r="B361" s="38" t="s">
         <v>191</v>
@@ -39788,7 +39787,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="362" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="38"/>
       <c r="B362" s="38" t="s">
         <v>191</v>
@@ -39864,7 +39863,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="363" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="38"/>
       <c r="B363" s="38" t="s">
         <v>191</v>
@@ -39940,7 +39939,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="364" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="38"/>
       <c r="B364" s="38" t="s">
         <v>191</v>
@@ -40030,7 +40029,7 @@
         <v>96571</v>
       </c>
     </row>
-    <row r="365" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="38"/>
       <c r="B365" s="38" t="s">
         <v>191</v>
@@ -40118,7 +40117,7 @@
         <v>124429</v>
       </c>
     </row>
-    <row r="366" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="38"/>
       <c r="B366" s="38" t="s">
         <v>191</v>
@@ -40204,7 +40203,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="367" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="38"/>
       <c r="B367" s="38" t="s">
         <v>191</v>
@@ -40290,7 +40289,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="368" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="38"/>
       <c r="B368" s="38" t="s">
         <v>191</v>
@@ -40376,7 +40375,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="369" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="38"/>
       <c r="B369" s="38" t="s">
         <v>191</v>
@@ -40598,7 +40597,7 @@
         <v>8409494051</v>
       </c>
     </row>
-    <row r="372" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="38"/>
       <c r="B372" s="38" t="s">
         <v>187</v>
@@ -40675,7 +40674,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="373" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="38"/>
       <c r="B373" s="38" t="s">
         <v>187</v>
@@ -40752,7 +40751,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="374" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="38"/>
       <c r="B374" s="38" t="s">
         <v>187</v>
@@ -40829,7 +40828,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="375" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="38"/>
       <c r="B375" s="38" t="s">
         <v>187</v>
@@ -40906,7 +40905,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="376" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="38"/>
       <c r="B376" s="38" t="s">
         <v>187</v>
@@ -40983,7 +40982,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="377" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="38"/>
       <c r="B377" s="38" t="s">
         <v>187</v>
@@ -41060,7 +41059,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="378" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="38"/>
       <c r="B378" s="38" t="s">
         <v>187</v>
@@ -41137,7 +41136,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="379" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="38"/>
       <c r="B379" s="38" t="s">
         <v>187</v>
@@ -41212,7 +41211,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="380" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="38"/>
       <c r="B380" s="38" t="s">
         <v>187</v>
@@ -41289,7 +41288,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="381" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A381" s="38"/>
       <c r="B381" s="38" t="s">
         <v>187</v>
@@ -41366,7 +41365,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="382" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A382" s="38"/>
       <c r="B382" s="38" t="s">
         <v>187</v>
@@ -41456,7 +41455,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="383" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A383" s="38"/>
       <c r="B383" s="38" t="s">
         <v>187</v>
@@ -41544,7 +41543,7 @@
         <v>84500</v>
       </c>
     </row>
-    <row r="384" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="38"/>
       <c r="B384" s="38" t="s">
         <v>187</v>
@@ -41631,7 +41630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="38"/>
       <c r="B385" s="38" t="s">
         <v>187</v>
@@ -41718,7 +41717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="38"/>
       <c r="B386" s="38" t="s">
         <v>187</v>
@@ -41805,7 +41804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="38"/>
       <c r="B387" s="38" t="s">
         <v>187</v>
@@ -42030,7 +42029,7 @@
         <v>8444651087</v>
       </c>
     </row>
-    <row r="390" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="38"/>
       <c r="B390" s="38" t="s">
         <v>182</v>
@@ -42106,7 +42105,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="391" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="38"/>
       <c r="B391" s="38" t="s">
         <v>182</v>
@@ -42182,7 +42181,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="392" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="38"/>
       <c r="B392" s="38" t="s">
         <v>182</v>
@@ -42258,7 +42257,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="393" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="38"/>
       <c r="B393" s="38" t="s">
         <v>182</v>
@@ -42334,7 +42333,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="394" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="38"/>
       <c r="B394" s="38" t="s">
         <v>182</v>
@@ -42410,7 +42409,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="395" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="38"/>
       <c r="B395" s="38" t="s">
         <v>182</v>
@@ -42486,7 +42485,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="396" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="38"/>
       <c r="B396" s="38" t="s">
         <v>182</v>
@@ -42562,7 +42561,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="397" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="38"/>
       <c r="B397" s="38" t="s">
         <v>182</v>
@@ -42710,7 +42709,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="399" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="38"/>
       <c r="B399" s="38" t="s">
         <v>182</v>
@@ -42783,7 +42782,7 @@
         <v>8460831345</v>
       </c>
     </row>
-    <row r="400" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="38"/>
       <c r="B400" s="38" t="s">
         <v>182</v>
@@ -42868,7 +42867,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="401" spans="1:29" s="15" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:29" s="15" customFormat="1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="38"/>
       <c r="B401" s="38" t="s">
         <v>182</v>
@@ -43326,11 +43325,11 @@
       <c r="O414" s="70"/>
       <c r="P414" s="14">
         <f>SUBTOTAL(109,P7:P413)</f>
-        <v>61316018</v>
+        <v>4452153</v>
       </c>
       <c r="Q414" s="14">
         <f>SUBTOTAL(109,Q7:Q413)</f>
-        <v>7816452</v>
+        <v>578780</v>
       </c>
       <c r="R414" s="46"/>
       <c r="S414" s="46"/>
@@ -44794,9 +44793,9 @@
     <row r="453" spans="8:44" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="B6:AR413" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="7">
+    <filterColumn colId="6">
       <filters>
-        <filter val="Tény"/>
+        <filter val="2023.04"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -44811,7 +44810,7 @@
       <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:AV400" xr:uid="{18C99A15-FB01-4B46-9E64-60BC60683E4E}">
+      <autoFilter ref="A4:AV400" xr:uid="{0B626DB0-8CD1-4D74-AD35-57E0B9B2F4EF}">
         <filterColumn colId="6">
           <filters>
             <filter val="2019.06"/>
@@ -45580,7 +45579,7 @@
       <selection activeCell="L44" sqref="L44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A41:N455" xr:uid="{B515244F-416C-4FBA-BA07-775E8C69740F}"/>
+      <autoFilter ref="A41:N455" xr:uid="{358FC013-0799-48B6-9A83-8EB919F776E7}"/>
     </customSheetView>
   </customSheetViews>
   <dataValidations count="6">

</xml_diff>